<commit_message>
major update, renaming of columns, separation of Fasta filtering from AAIMON ratio calculation, improvement of fasta filtering, update of settings file
</commit_message>
<xml_diff>
--- a/korbinian/settings/korbinian_run_settings_schweris.xlsx
+++ b/korbinian/settings/korbinian_run_settings_schweris.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="174">
   <si>
     <t>uniprot_list</t>
   </si>
@@ -117,69 +117,15 @@
     <t>overwrite_csv_file_av_cons_ratios_hits</t>
   </si>
   <si>
-    <t>e_value_filter</t>
-  </si>
-  <si>
-    <t>words_not_allowed_in_description</t>
-  </si>
-  <si>
     <t>["patent","Patent","synthetic","Synthetic","artificial","Artificial","bad sequence","low quality"]</t>
   </si>
   <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>number_of_gaps_allowed_in_match_TMD</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
-    <t>number_of_gaps_allowed_in_query_TMD</t>
-  </si>
-  <si>
-    <t>minimum_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>min_identity_of_TMD_initial_filter</t>
-  </si>
-  <si>
-    <t>min_identity_of_TMD_final_filter</t>
-  </si>
-  <si>
-    <t>number_of_X_allowed_in_TMD</t>
-  </si>
-  <si>
-    <t>number_of_X_allowed_in_seq</t>
-  </si>
-  <si>
-    <t>min_len_query_aln_seq_excl_TMD</t>
-  </si>
-  <si>
-    <t>identity_method</t>
-  </si>
-  <si>
     <t>gappedIdentity</t>
   </si>
   <si>
-    <t>maximum_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>mimimum_length_match_sequence</t>
-  </si>
-  <si>
-    <t>mimimum_length_non_TMD_sequence</t>
-  </si>
-  <si>
-    <t>randomised_tmd</t>
-  </si>
-  <si>
-    <t>aa_before_tmd</t>
-  </si>
-  <si>
-    <t>aa_after_tmd</t>
-  </si>
-  <si>
     <t>suppress_error_logging_to_console</t>
   </si>
   <si>
@@ -303,9 +249,6 @@
     <t xml:space="preserve">Java Executable String (usually "java", or %JAVAJRE%, depending on java_home settings in Windows). </t>
   </si>
   <si>
-    <t>SIMAP homologue filtering for fasta output</t>
-  </si>
-  <si>
     <t>UniProt non-redundancy parameters</t>
   </si>
   <si>
@@ -493,6 +436,108 @@
   </si>
   <si>
     <t>mp_xlim_max01</t>
+  </si>
+  <si>
+    <t>fa_words_not_allowed_in_description</t>
+  </si>
+  <si>
+    <t>fa_database</t>
+  </si>
+  <si>
+    <t>fa_min_identity_of_TMD_initial_filter</t>
+  </si>
+  <si>
+    <t>fa_min_identity_of_TMD_final_filter</t>
+  </si>
+  <si>
+    <t>fa_identity_method</t>
+  </si>
+  <si>
+    <t>fa_randomised_tmd</t>
+  </si>
+  <si>
+    <t>fa_aa_before_tmd</t>
+  </si>
+  <si>
+    <t>fa_aa_after_tmd</t>
+  </si>
+  <si>
+    <t>fa_X_allowed_in_sel_seq</t>
+  </si>
+  <si>
+    <t>cr_words_not_allowed_in_description</t>
+  </si>
+  <si>
+    <t>cr_database</t>
+  </si>
+  <si>
+    <t>cr_minimum_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_min_identity_of_TMD_initial_filter</t>
+  </si>
+  <si>
+    <t>cr_min_identity_of_TMD_final_filter</t>
+  </si>
+  <si>
+    <t>cr_X_allowed_in_full_seq</t>
+  </si>
+  <si>
+    <t>cr_min_len_query_aln_seq_excl_TMD</t>
+  </si>
+  <si>
+    <t>cr_identity_method</t>
+  </si>
+  <si>
+    <t>cr_maximum_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_mimimum_length_match_sequence</t>
+  </si>
+  <si>
+    <t>cr_mimimum_length_non_TMD_sequence</t>
+  </si>
+  <si>
+    <t>cr_randomised_tmd</t>
+  </si>
+  <si>
+    <t>fa_X_allowed_in_full_seq</t>
+  </si>
+  <si>
+    <t>fa_max_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>fa_min_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_max_n_gaps_in_match_TMD</t>
+  </si>
+  <si>
+    <t>cr_max_n_gaps_in_query_TMD</t>
+  </si>
+  <si>
+    <t>fa_max_n_gaps_in_match_TMD</t>
+  </si>
+  <si>
+    <t>fa_max_n_gaps_in_query_TMD</t>
+  </si>
+  <si>
+    <t>remove_redundant_seqs</t>
+  </si>
+  <si>
+    <t>add_query_seq</t>
+  </si>
+  <si>
+    <t>save_fasta_plus_surr</t>
+  </si>
+  <si>
+    <t>save a second fasta output with the TMD or selected sequence plus the surrounding sequence</t>
+  </si>
+  <si>
+    <t>SIMAP homologue filtering for conservation ratio (cr) output</t>
+  </si>
+  <si>
+    <t>SIMAP homologue filtering for fasta (fa) output</t>
   </si>
 </sst>
 </file>
@@ -524,7 +569,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -651,6 +696,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF868E1A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F8BA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -664,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -816,11 +873,32 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1040,6 +1118,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF4F8BA"/>
+      <color rgb="FF868E1A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1337,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,18 +1435,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -1405,14 +1489,14 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>8</v>
@@ -1423,7 +1507,7 @@
     </row>
     <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B9" s="70" t="s">
         <v>8</v>
@@ -1434,7 +1518,7 @@
     </row>
     <row r="10" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>8</v>
@@ -1445,7 +1529,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B11" s="70" t="s">
         <v>8</v>
@@ -1456,7 +1540,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B12" s="70" t="s">
         <v>8</v>
@@ -1467,7 +1551,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>8</v>
@@ -1482,14 +1566,14 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="57"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B16" s="70" t="s">
         <v>8</v>
@@ -1500,7 +1584,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B17" s="70" t="s">
         <v>8</v>
@@ -1515,31 +1599,31 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>7</v>
+        <v>110</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1549,28 +1633,28 @@
     </row>
     <row r="23" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="60"/>
     </row>
     <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B24" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>7</v>
+        <v>112</v>
+      </c>
+      <c r="B25" s="70" t="s">
+        <v>8</v>
       </c>
       <c r="C25" s="61" t="s">
         <v>20</v>
@@ -1578,7 +1662,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B26" s="70" t="s">
         <v>8</v>
@@ -1593,14 +1677,14 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>8</v>
@@ -1611,7 +1695,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B30" s="70" t="s">
         <v>8</v>
@@ -1622,7 +1706,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B31" s="70" t="s">
         <v>8</v>
@@ -1633,7 +1717,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B32" s="70" t="s">
         <v>8</v>
@@ -1644,7 +1728,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B33" s="70" t="s">
         <v>8</v>
@@ -1655,7 +1739,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B34" s="70" t="s">
         <v>8</v>
@@ -1666,48 +1750,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B6 B35:B1048576">
-    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="37" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="35" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="23" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="34" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="32" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B34 B24 B26 B8:B13 B16:B17">
-    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B29:B34 B24 B26 B8:B10 B16">
+    <cfRule type="containsText" dxfId="6" priority="31" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="5" priority="23" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
+  <conditionalFormatting sqref="B17 B11:B13">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1732,13 +1821,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1746,7 +1835,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1754,82 +1843,82 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1840,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,18 +1944,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -1894,10 +1983,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1908,7 +1997,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1917,7 +2006,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
@@ -1960,18 +2049,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B13" s="40">
         <v>5000</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B14" s="40">
         <v>1.0000000000000001E-5</v>
@@ -1980,7 +2069,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B15" s="40">
         <v>5000</v>
@@ -1989,7 +2078,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B16" s="40">
         <v>3000</v>
@@ -1998,7 +2087,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>8</v>
@@ -2007,10 +2096,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C18" s="56"/>
     </row>
@@ -2020,554 +2109,648 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="57"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="42">
-        <v>1.0000000000000001E-5</v>
+        <v>169</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>7</v>
       </c>
       <c r="C21" s="58"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C22" s="58"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="58"/>
+        <v>7</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="B24" s="42">
         <v>2</v>
       </c>
-      <c r="C24" s="58">
-        <v>2</v>
-      </c>
+      <c r="C24" s="58"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="B25" s="42">
         <v>2</v>
       </c>
-      <c r="C25" s="58">
-        <v>2</v>
-      </c>
+      <c r="C25" s="58"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="C26" s="58">
-        <v>0.7</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="58"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="B27" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="C27" s="58">
-        <v>0.2</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="C27" s="58"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B28" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="C28" s="58">
-        <v>0.2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C28" s="58"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="B29" s="42">
-        <v>0</v>
-      </c>
-      <c r="C29" s="58">
-        <v>0</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="C29" s="58"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="B30" s="42">
-        <v>20</v>
-      </c>
-      <c r="C30" s="58">
-        <v>0</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="C30" s="58"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="42">
-        <v>20</v>
-      </c>
-      <c r="C31" s="58">
-        <v>20</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="58"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="58" t="s">
-        <v>47</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="42">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C33" s="58">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="B34" s="42">
-        <v>0</v>
-      </c>
-      <c r="C34" s="58">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="B35" s="42">
-        <v>0</v>
-      </c>
-      <c r="C35" s="58">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C35" s="58"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="58" t="s">
-        <v>8</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C36" s="58"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="42">
-        <v>10</v>
-      </c>
-      <c r="C37" s="58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="42">
-        <v>10</v>
-      </c>
-      <c r="C38" s="58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="38"/>
-      <c r="C39" s="8"/>
+        <v>141</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="58"/>
+    </row>
+    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="38"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="72"/>
+      <c r="C39" s="73"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="59"/>
+      <c r="A40" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="76"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="44" t="s">
+      <c r="A41" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="76"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="75">
+        <v>2</v>
+      </c>
+      <c r="C42" s="76"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="75">
+        <v>2</v>
+      </c>
+      <c r="C43" s="76"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="75">
+        <v>0.4</v>
+      </c>
+      <c r="C44" s="76"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="75">
+        <v>0.3</v>
+      </c>
+      <c r="C45" s="76"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="75">
+        <v>0.3</v>
+      </c>
+      <c r="C46" s="76"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="76"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="75">
+        <v>20</v>
+      </c>
+      <c r="C48" s="76"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="B49" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="76"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="75">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C50" s="76"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="75">
+        <v>0</v>
+      </c>
+      <c r="C51" s="76"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="75">
+        <v>0</v>
+      </c>
+      <c r="C52" s="76"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="76"/>
+    </row>
+    <row r="54" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="38"/>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="43"/>
+      <c r="C55" s="59"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="44">
+      <c r="C56" s="25"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="44">
         <v>2</v>
       </c>
-      <c r="C42" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="44">
+      <c r="C57" s="25"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="44">
         <v>24</v>
       </c>
-      <c r="C43" s="25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="44">
+      <c r="C58" s="25"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="44">
         <v>20</v>
       </c>
-      <c r="C44" s="25"/>
-    </row>
-    <row r="45" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="38"/>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="60"/>
-    </row>
-    <row r="47" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="46">
+      <c r="C59" s="25"/>
+    </row>
+    <row r="60" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="38"/>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="45"/>
+      <c r="C61" s="60"/>
+    </row>
+    <row r="62" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="46">
         <v>30</v>
       </c>
-      <c r="C47" s="61"/>
-    </row>
-    <row r="48" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B48" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="61"/>
-    </row>
-    <row r="49" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="46">
-        <v>3.05</v>
-      </c>
-      <c r="C49" s="61"/>
-    </row>
-    <row r="50" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B50" s="46">
-        <v>20</v>
-      </c>
-      <c r="C50" s="61"/>
-    </row>
-    <row r="51" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="46">
-        <v>31</v>
-      </c>
-      <c r="C51" s="61"/>
-    </row>
-    <row r="52" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="61"/>
-    </row>
-    <row r="53" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="61"/>
-    </row>
-    <row r="54" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="46">
-        <v>0.05</v>
-      </c>
-      <c r="C54" s="61"/>
-    </row>
-    <row r="55" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="46">
-        <v>3</v>
-      </c>
-      <c r="C55" s="61"/>
-    </row>
-    <row r="56" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="61"/>
-    </row>
-    <row r="57" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="46">
-        <v>1.4550000000000001</v>
-      </c>
-      <c r="C57" s="61"/>
-    </row>
-    <row r="58" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" s="46">
-        <v>31</v>
-      </c>
-      <c r="C58" s="61"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="61"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="46">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="C60" s="61"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="B61" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="C61" s="61"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="46">
-        <v>1.75</v>
-      </c>
       <c r="C62" s="61"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B63" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="61"/>
     </row>
-    <row r="65" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="48"/>
-      <c r="C65" s="27"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="49">
+    <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="46">
+        <v>3.05</v>
+      </c>
+      <c r="C64" s="61"/>
+    </row>
+    <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="46">
+        <v>20</v>
+      </c>
+      <c r="C65" s="61"/>
+    </row>
+    <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="46">
+        <v>31</v>
+      </c>
+      <c r="C66" s="61"/>
+    </row>
+    <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="61"/>
+    </row>
+    <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="61"/>
+    </row>
+    <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="C69" s="61"/>
+    </row>
+    <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70" s="46">
+        <v>3</v>
+      </c>
+      <c r="C70" s="61"/>
+    </row>
+    <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="61"/>
+    </row>
+    <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="46">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="C72" s="61"/>
+    </row>
+    <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="46">
+        <v>31</v>
+      </c>
+      <c r="C73" s="61"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="61"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="46">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="C75" s="61"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C76" s="61"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="46">
+        <v>1.75</v>
+      </c>
+      <c r="C77" s="61"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="61"/>
+    </row>
+    <row r="80" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="48"/>
+      <c r="C80" s="27"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B81" s="49">
         <v>0</v>
       </c>
-      <c r="C66" s="29"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="49">
+      <c r="C81" s="29"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82" s="49">
         <v>-12</v>
       </c>
-      <c r="C67" s="29"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" s="49">
+      <c r="C82" s="29"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="49">
         <v>-2</v>
       </c>
-      <c r="C68" s="29"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="29"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B70" s="49">
+      <c r="C83" s="29"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C84" s="29"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" s="49">
         <v>-0.2</v>
       </c>
-      <c r="C70" s="29"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="49">
+      <c r="C85" s="29"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B86" s="49">
         <v>-1</v>
       </c>
-      <c r="C71" s="29"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="49">
+      <c r="C86" s="29"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" s="49">
         <v>-1</v>
       </c>
-      <c r="C72" s="29"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="49">
+      <c r="C87" s="29"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B88" s="49">
         <v>0</v>
       </c>
-      <c r="C73" s="29"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B74" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="29"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B76" s="50"/>
-      <c r="C76" s="30"/>
-    </row>
-    <row r="77" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B77" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="33"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B78" s="51">
+      <c r="C88" s="29"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C89" s="29"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="50"/>
+      <c r="C91" s="30"/>
+    </row>
+    <row r="92" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="33"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" s="51">
         <v>5</v>
       </c>
-      <c r="C78" s="33"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B79" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="33"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B80" s="51" t="s">
+      <c r="C93" s="33"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C80" s="51"/>
+      <c r="B94" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="33"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B95" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C95" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added filter "X" for TMD plus surr
</commit_message>
<xml_diff>
--- a/korbinian/settings/korbinian_run_settings_schweris.xlsx
+++ b/korbinian/settings/korbinian_run_settings_schweris.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="177">
   <si>
     <t>uniprot_list</t>
   </si>
@@ -538,6 +538,15 @@
   </si>
   <si>
     <t>SIMAP homologue filtering for fasta (fa) output</t>
+  </si>
+  <si>
+    <t>filter_selected_seq_based_on_hydrophobicity</t>
+  </si>
+  <si>
+    <t>max_hydrophilicity_Hessa</t>
+  </si>
+  <si>
+    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment.</t>
   </si>
 </sst>
 </file>
@@ -891,147 +900,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1422,7 +1291,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1678,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,88 +2014,90 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="42">
-        <v>2</v>
+        <v>174</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>7</v>
       </c>
       <c r="C24" s="58"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B25" s="42">
-        <v>2</v>
-      </c>
-      <c r="C25" s="58"/>
+        <v>-1</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>35</v>
+        <v>166</v>
+      </c>
+      <c r="B26" s="42">
+        <v>10</v>
       </c>
       <c r="C26" s="58"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B27" s="42">
-        <v>0.4</v>
+        <v>10</v>
       </c>
       <c r="C27" s="58"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="42">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="C28" s="58"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="B29" s="42">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C29" s="58"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B30" s="42">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C30" s="58"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="B31" s="42" t="s">
-        <v>8</v>
+        <v>142</v>
+      </c>
+      <c r="B31" s="42">
+        <v>0.3</v>
       </c>
       <c r="C31" s="58"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="42" t="s">
-        <v>8</v>
+        <v>143</v>
+      </c>
+      <c r="B32" s="42">
+        <v>0.3</v>
       </c>
       <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>8</v>
@@ -2235,518 +2106,536 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B34" s="42">
-        <v>10</v>
+        <v>148</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B35" s="42">
-        <v>10</v>
+        <v>145</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="C35" s="58"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>33</v>
+        <v>146</v>
+      </c>
+      <c r="B36" s="42">
+        <v>10</v>
       </c>
       <c r="C36" s="58"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="42">
+        <v>10</v>
+      </c>
+      <c r="C37" s="58"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="58"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B39" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="58"/>
-    </row>
-    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="38"/>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="71" t="s">
+      <c r="C39" s="58"/>
+    </row>
+    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="38"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="73"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="B40" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="76"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="76"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
-        <v>164</v>
-      </c>
-      <c r="B42" s="75">
-        <v>2</v>
+        <v>149</v>
+      </c>
+      <c r="B42" s="75" t="s">
+        <v>33</v>
       </c>
       <c r="C42" s="76"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" s="75">
-        <v>2</v>
+        <v>150</v>
+      </c>
+      <c r="B43" s="75" t="s">
+        <v>34</v>
       </c>
       <c r="C43" s="76"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B44" s="75">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="C44" s="76"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B45" s="75">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="76"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B46" s="75">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C46" s="76"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="B47" s="75" t="s">
-        <v>8</v>
+        <v>152</v>
+      </c>
+      <c r="B47" s="75">
+        <v>0.3</v>
       </c>
       <c r="C47" s="76"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B48" s="75">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="C48" s="76"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B49" s="75" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C49" s="76"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B50" s="75">
-        <v>1.1000000000000001</v>
+        <v>20</v>
       </c>
       <c r="C50" s="76"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="B51" s="75">
-        <v>0</v>
+        <v>156</v>
+      </c>
+      <c r="B51" s="75" t="s">
+        <v>35</v>
       </c>
       <c r="C51" s="76"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B52" s="75">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C52" s="76"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="75">
+        <v>0</v>
+      </c>
+      <c r="C53" s="76"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="75">
+        <v>0</v>
+      </c>
+      <c r="C54" s="76"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="76"/>
-    </row>
-    <row r="54" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="38"/>
-      <c r="C54" s="8"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+      <c r="B55" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="76"/>
+    </row>
+    <row r="56" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="38"/>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="59"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="25"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="44">
-        <v>2</v>
-      </c>
-      <c r="C57" s="25"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="59"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="44">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>7</v>
       </c>
       <c r="C58" s="25"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="44">
+        <v>2</v>
+      </c>
+      <c r="C59" s="25"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="44">
+        <v>24</v>
+      </c>
+      <c r="C60" s="25"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="44">
+      <c r="B61" s="44">
         <v>20</v>
       </c>
-      <c r="C59" s="25"/>
-    </row>
-    <row r="60" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="38"/>
-      <c r="C60" s="8"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="C61" s="25"/>
+    </row>
+    <row r="62" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="38"/>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="45"/>
-      <c r="C61" s="60"/>
-    </row>
-    <row r="62" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62" s="46">
-        <v>30</v>
-      </c>
-      <c r="C62" s="61"/>
-    </row>
-    <row r="63" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="61"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="60"/>
     </row>
     <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" s="46">
-        <v>3.05</v>
+        <v>30</v>
       </c>
       <c r="C64" s="61"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B65" s="46">
-        <v>20</v>
+        <v>84</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C65" s="61"/>
     </row>
     <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66" s="46">
-        <v>31</v>
+        <v>3.05</v>
       </c>
       <c r="C66" s="61"/>
     </row>
     <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B67" s="46" t="s">
-        <v>7</v>
+        <v>120</v>
+      </c>
+      <c r="B67" s="46">
+        <v>20</v>
       </c>
       <c r="C67" s="61"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68" s="46" t="s">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="B68" s="46">
+        <v>31</v>
       </c>
       <c r="C68" s="61"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B69" s="46">
-        <v>0.05</v>
+        <v>87</v>
+      </c>
+      <c r="B69" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B70" s="46">
-        <v>3</v>
+        <v>88</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>8</v>
       </c>
       <c r="C70" s="61"/>
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B71" s="46" t="s">
-        <v>7</v>
+        <v>89</v>
+      </c>
+      <c r="B71" s="46">
+        <v>0.05</v>
       </c>
       <c r="C71" s="61"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B72" s="46">
-        <v>1.4550000000000001</v>
+        <v>3</v>
       </c>
       <c r="C72" s="61"/>
     </row>
     <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="61"/>
+    </row>
+    <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="46">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="C74" s="61"/>
+    </row>
+    <row r="75" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="46">
+      <c r="B75" s="46">
         <v>31</v>
-      </c>
-      <c r="C73" s="61"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B74" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="61"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B75" s="46">
-        <v>0.55500000000000005</v>
       </c>
       <c r="C75" s="61"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" s="46">
-        <v>0.5</v>
+        <v>94</v>
+      </c>
+      <c r="B76" s="46" t="s">
+        <v>8</v>
       </c>
       <c r="C76" s="61"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B77" s="46">
-        <v>1.75</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C77" s="61"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C78" s="61"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" s="46">
+        <v>1.75</v>
+      </c>
+      <c r="C79" s="61"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B78" s="46" t="s">
+      <c r="B80" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="61"/>
-    </row>
-    <row r="80" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="26" t="s">
+      <c r="C80" s="61"/>
+    </row>
+    <row r="82" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="48"/>
-      <c r="C80" s="27"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" s="49">
-        <v>0</v>
-      </c>
-      <c r="C81" s="29"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B82" s="49">
-        <v>-12</v>
-      </c>
-      <c r="C82" s="29"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B83" s="49">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C83" s="29"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B84" s="49" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="B84" s="49">
+        <v>-12</v>
       </c>
       <c r="C84" s="29"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B85" s="49">
-        <v>-0.2</v>
+        <v>-2</v>
       </c>
       <c r="C85" s="29"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B86" s="49">
-        <v>-1</v>
+        <v>43</v>
+      </c>
+      <c r="B86" s="49" t="s">
+        <v>48</v>
       </c>
       <c r="C86" s="29"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B87" s="49">
-        <v>-1</v>
+        <v>-0.2</v>
       </c>
       <c r="C87" s="29"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B88" s="49">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C88" s="29"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" s="49">
+        <v>-1</v>
+      </c>
+      <c r="C89" s="29"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B90" s="49">
+        <v>0</v>
+      </c>
+      <c r="C90" s="29"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B89" s="49" t="s">
+      <c r="B91" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C89" s="29"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="34" t="s">
+      <c r="C91" s="29"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B91" s="50"/>
-      <c r="C91" s="30"/>
-    </row>
-    <row r="92" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+      <c r="B93" s="50"/>
+      <c r="C93" s="30"/>
+    </row>
+    <row r="94" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B92" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" s="33"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B93" s="51">
-        <v>5</v>
-      </c>
-      <c r="C93" s="33"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="B94" s="51" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C94" s="33"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" s="51">
+        <v>5</v>
+      </c>
+      <c r="C95" s="33"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B96" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C96" s="33"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B95" s="51" t="s">
+      <c r="B97" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C95" s="51"/>
+      <c r="C97" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">

</xml_diff>

<commit_message>
added settings file for server, and function to move SIMAP data folders
</commit_message>
<xml_diff>
--- a/korbinian/settings/korbinian_run_settings_schweris.xlsx
+++ b/korbinian/settings/korbinian_run_settings_schweris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="3090" yWindow="2775" windowWidth="14265" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="186">
   <si>
     <t>uniprot_list</t>
   </si>
@@ -66,9 +66,6 @@
     <t>If "TRUE", the uniprot flatfile will be parsed into a csv file (List##_uniprot.csv), extracting fields of interest such as the full sequence, the transmembrane domain sequences, protein description, protein keywords, disease mutations, etc.</t>
   </si>
   <si>
-    <t>If "TRUE", the data types of the csv file will be corrected.</t>
-  </si>
-  <si>
     <t>If "TRUE", the file locations for that protein will be appended to the csv file.</t>
   </si>
   <si>
@@ -234,183 +231,336 @@
     <t>eaSimap_path</t>
   </si>
   <si>
+    <t>r'/nas/teeselab/programs/eaSimap.jar'</t>
+  </si>
+  <si>
+    <t>java_exec_str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Executable String (usually "java", or %JAVAJRE%, depending on java_home settings in Windows). </t>
+  </si>
+  <si>
+    <t>UniProt non-redundancy parameters</t>
+  </si>
+  <si>
+    <t>SIMAP homologue download parameters</t>
+  </si>
+  <si>
+    <t>Gap analysis parameters</t>
+  </si>
+  <si>
+    <t>TMD/nonTMD conservation analysis parameters</t>
+  </si>
+  <si>
+    <t>Old parameters, no longer in use</t>
+  </si>
+  <si>
+    <t>Amino acid substitution scoring parameters</t>
+  </si>
+  <si>
+    <t>1p_final_highest_bin</t>
+  </si>
+  <si>
+    <t>1p_fixed_bins</t>
+  </si>
+  <si>
+    <t>1p_largest_bin</t>
+  </si>
+  <si>
+    <t>1p_number_of_bins</t>
+  </si>
+  <si>
+    <t>1p_overwrite_histogram_files</t>
+  </si>
+  <si>
+    <t>1p_pylab_automatic_bins</t>
+  </si>
+  <si>
+    <t>1p_smallest_bin</t>
+  </si>
+  <si>
+    <t>mp_final_highest_bin</t>
+  </si>
+  <si>
+    <t>mp_fixed_bins</t>
+  </si>
+  <si>
+    <t>mp_largest_bin</t>
+  </si>
+  <si>
+    <t>mp_number_of_bins</t>
+  </si>
+  <si>
+    <t>mp_pylab_automatic_bins</t>
+  </si>
+  <si>
+    <t>mp_smallest_bin</t>
+  </si>
+  <si>
+    <t>UniProt run settings</t>
+  </si>
+  <si>
+    <t>SIMAP run settings</t>
+  </si>
+  <si>
+    <t>Analysis run settings</t>
+  </si>
+  <si>
+    <t>TMD/nonTMD conservation plotting run settings</t>
+  </si>
+  <si>
+    <t>Old run settings</t>
+  </si>
+  <si>
+    <t>run_parse_large_flatfile_with_list_uniprot_accessions</t>
+  </si>
+  <si>
+    <t>run_retrieve_uniprot_data_for_acc_list_in_xlsx_file</t>
+  </si>
+  <si>
+    <t>run_convert_uniprot_list_to_nonred_ff_via_uniref</t>
+  </si>
+  <si>
+    <t>run_create_csv_from_uniprot_flatfile</t>
+  </si>
+  <si>
+    <t>run_retrieve_simap_feature_table_and_homologues_from_list_in_csv</t>
+  </si>
+  <si>
+    <t>run_parse_simap_to_csv</t>
+  </si>
+  <si>
+    <t>run_calculate_AAIMON_ratios</t>
+  </si>
+  <si>
+    <t>run_calculate_gap_densities</t>
+  </si>
+  <si>
+    <t>run_create_graph_of_gap_density</t>
+  </si>
+  <si>
+    <t>run_save_figures_describing_proteins_in_list</t>
+  </si>
+  <si>
+    <t>run_compare_lists</t>
+  </si>
+  <si>
+    <t>old_calculate_TMD_conservation</t>
+  </si>
+  <si>
+    <t>old_calculate_TMD_conservation_by_gappedIdentity</t>
+  </si>
+  <si>
+    <t>old_calculate_TMD_conservation_moment</t>
+  </si>
+  <si>
+    <t>old_conduct_stat_analysis_with_all_seqs_or_nonredundant_seqs</t>
+  </si>
+  <si>
+    <t>old_fix_dfout05_simapcsv_by_adding_query_md5</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>1p_min_n_hits_for_data_analysis</t>
+  </si>
+  <si>
+    <t>old_run_stat_analysis_sim_ratios_in_dfout05</t>
+  </si>
+  <si>
+    <t>stat_analysis_all_seqs_or_nonred_seqs</t>
+  </si>
+  <si>
+    <t>Protein lists chosen for analysis</t>
+  </si>
+  <si>
+    <t>D:\</t>
+  </si>
+  <si>
+    <t>D:\Databases</t>
+  </si>
+  <si>
+    <t>D:\Databases\main</t>
+  </si>
+  <si>
+    <t>list_of_uniprot_accessions</t>
+  </si>
+  <si>
+    <t>D:\Databases\main\input_acc_lists\List01_uniprot_accessions.txt</t>
+  </si>
+  <si>
+    <t>aa_sub_matrices</t>
+  </si>
+  <si>
+    <t>mp_xlim_min01</t>
+  </si>
+  <si>
+    <t>mp_xlim_max01</t>
+  </si>
+  <si>
+    <t>fa_words_not_allowed_in_description</t>
+  </si>
+  <si>
+    <t>fa_database</t>
+  </si>
+  <si>
+    <t>fa_identity_method</t>
+  </si>
+  <si>
+    <t>fa_aa_before_tmd</t>
+  </si>
+  <si>
+    <t>fa_aa_after_tmd</t>
+  </si>
+  <si>
+    <t>fa_X_allowed_in_sel_seq</t>
+  </si>
+  <si>
+    <t>cr_words_not_allowed_in_description</t>
+  </si>
+  <si>
+    <t>cr_database</t>
+  </si>
+  <si>
+    <t>cr_minimum_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_min_identity_of_TMD_initial_filter</t>
+  </si>
+  <si>
+    <t>cr_min_identity_of_TMD_final_filter</t>
+  </si>
+  <si>
+    <t>cr_X_allowed_in_full_seq</t>
+  </si>
+  <si>
+    <t>cr_min_len_query_aln_seq_excl_TMD</t>
+  </si>
+  <si>
+    <t>cr_identity_method</t>
+  </si>
+  <si>
+    <t>cr_maximum_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_mimimum_length_match_sequence</t>
+  </si>
+  <si>
+    <t>cr_mimimum_length_non_TMD_sequence</t>
+  </si>
+  <si>
+    <t>cr_randomised_tmd</t>
+  </si>
+  <si>
+    <t>fa_X_allowed_in_full_seq</t>
+  </si>
+  <si>
+    <t>fa_max_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>fa_min_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>cr_max_n_gaps_in_match_TMD</t>
+  </si>
+  <si>
+    <t>cr_max_n_gaps_in_query_TMD</t>
+  </si>
+  <si>
+    <t>fa_max_n_gaps_in_match_TMD</t>
+  </si>
+  <si>
+    <t>fa_max_n_gaps_in_query_TMD</t>
+  </si>
+  <si>
+    <t>remove_redundant_seqs</t>
+  </si>
+  <si>
+    <t>add_query_seq</t>
+  </si>
+  <si>
+    <t>save_fasta_plus_surr</t>
+  </si>
+  <si>
+    <t>save a second fasta output with the TMD or selected sequence plus the surrounding sequence</t>
+  </si>
+  <si>
+    <t>SIMAP homologue filtering for conservation ratio (cr) output</t>
+  </si>
+  <si>
+    <t>SIMAP homologue filtering for fasta (fa) output</t>
+  </si>
+  <si>
+    <t>filter_selected_seq_based_on_hydrophobicity</t>
+  </si>
+  <si>
+    <t>max_hydrophilicity_Hessa</t>
+  </si>
+  <si>
+    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment.</t>
+  </si>
+  <si>
+    <t>your_name</t>
+  </si>
+  <si>
+    <t>Jakob Maria Mierscheid</t>
+  </si>
+  <si>
+    <t>ASCII text! Identifier to determine who downloaded SIMAP homologues</t>
+  </si>
+  <si>
+    <t>not used!</t>
+  </si>
+  <si>
+    <t>0.4 = 40% aa identity excluding gaps</t>
+  </si>
+  <si>
+    <t>1 = 100% aa identity excluding gaps</t>
+  </si>
+  <si>
+    <t>do you want the original query sequence to be the first seq of the homologues?</t>
+  </si>
+  <si>
+    <t>do you want redundant selected (e.g. TMD) sequences to be removed before saving to fasta</t>
+  </si>
+  <si>
+    <t>homol_dir</t>
+  </si>
+  <si>
+    <t>summaries_dir</t>
+  </si>
+  <si>
+    <t>simap_database_dir</t>
+  </si>
+  <si>
+    <t>uniprot_dir</t>
+  </si>
+  <si>
+    <t>directory with uniprot files</t>
+  </si>
+  <si>
+    <t>directory where the homologue output files and analysis will be found</t>
+  </si>
+  <si>
+    <t>run_setup_df_file_locations</t>
+  </si>
+  <si>
+    <t>logfile_dir</t>
+  </si>
+  <si>
+    <t>run_create_fasta</t>
+  </si>
+  <si>
+    <t>slice_juxtamembrane_regions</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
     <t>D:\Schweris\Projects\Programming\Python\programs\eaSimap.jar</t>
   </si>
   <si>
-    <t>r'/nas/teeselab/programs/eaSimap.jar'</t>
-  </si>
-  <si>
-    <t>java</t>
-  </si>
-  <si>
-    <t>java_exec_str</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java Executable String (usually "java", or %JAVAJRE%, depending on java_home settings in Windows). </t>
-  </si>
-  <si>
-    <t>UniProt non-redundancy parameters</t>
-  </si>
-  <si>
-    <t>SIMAP homologue download parameters</t>
-  </si>
-  <si>
-    <t>Gap analysis parameters</t>
-  </si>
-  <si>
-    <t>TMD/nonTMD conservation analysis parameters</t>
-  </si>
-  <si>
-    <t>Old parameters, no longer in use</t>
-  </si>
-  <si>
-    <t>Amino acid substitution scoring parameters</t>
-  </si>
-  <si>
-    <t>1p_final_highest_bin</t>
-  </si>
-  <si>
-    <t>1p_fixed_bins</t>
-  </si>
-  <si>
-    <t>1p_largest_bin</t>
-  </si>
-  <si>
-    <t>1p_number_of_bins</t>
-  </si>
-  <si>
-    <t>1p_overwrite_histogram_files</t>
-  </si>
-  <si>
-    <t>1p_pylab_automatic_bins</t>
-  </si>
-  <si>
-    <t>1p_smallest_bin</t>
-  </si>
-  <si>
-    <t>mp_final_highest_bin</t>
-  </si>
-  <si>
-    <t>mp_fixed_bins</t>
-  </si>
-  <si>
-    <t>mp_largest_bin</t>
-  </si>
-  <si>
-    <t>mp_number_of_bins</t>
-  </si>
-  <si>
-    <t>mp_pylab_automatic_bins</t>
-  </si>
-  <si>
-    <t>mp_smallest_bin</t>
-  </si>
-  <si>
-    <t>UniProt run settings</t>
-  </si>
-  <si>
-    <t>SIMAP run settings</t>
-  </si>
-  <si>
-    <t>Analysis run settings</t>
-  </si>
-  <si>
-    <t>TMD/nonTMD conservation plotting run settings</t>
-  </si>
-  <si>
-    <t>Old run settings</t>
-  </si>
-  <si>
-    <t>run_parse_large_flatfile_with_list_uniprot_accessions</t>
-  </si>
-  <si>
-    <t>run_retrieve_uniprot_data_for_acc_list_in_xlsx_file</t>
-  </si>
-  <si>
-    <t>run_convert_uniprot_list_to_nonred_ff_via_uniref</t>
-  </si>
-  <si>
-    <t>run_create_csv_from_uniprot_flatfile</t>
-  </si>
-  <si>
-    <t>run_A04_setup_df_dtypes</t>
-  </si>
-  <si>
-    <t>run_A05_setup_df_file_locations</t>
-  </si>
-  <si>
-    <t>run_retrieve_simap_feature_table_and_homologues_from_list_in_csv</t>
-  </si>
-  <si>
-    <t>run_parse_simap_to_csv</t>
-  </si>
-  <si>
-    <t>run_calculate_AAIMON_ratios</t>
-  </si>
-  <si>
-    <t>run_calculate_gap_densities</t>
-  </si>
-  <si>
-    <t>run_create_graph_of_gap_density</t>
-  </si>
-  <si>
-    <t>run_save_figures_describing_proteins_in_list</t>
-  </si>
-  <si>
-    <t>run_compare_lists</t>
-  </si>
-  <si>
-    <t>old_calculate_TMD_conservation</t>
-  </si>
-  <si>
-    <t>old_calculate_TMD_conservation_by_gappedIdentity</t>
-  </si>
-  <si>
-    <t>old_calculate_TMD_conservation_moment</t>
-  </si>
-  <si>
-    <t>old_conduct_stat_analysis_with_all_seqs_or_nonredundant_seqs</t>
-  </si>
-  <si>
-    <t>old_fix_dfout05_simapcsv_by_adding_query_md5</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>1p_min_n_hits_for_data_analysis</t>
-  </si>
-  <si>
-    <t>old_run_stat_analysis_sim_ratios_in_dfout05</t>
-  </si>
-  <si>
-    <t>stat_analysis_all_seqs_or_nonred_seqs</t>
-  </si>
-  <si>
-    <t>Protein lists chosen for analysis</t>
-  </si>
-  <si>
-    <t>D:\</t>
-  </si>
-  <si>
-    <t>D:\Databases</t>
-  </si>
-  <si>
-    <t>D:\Databases\main</t>
-  </si>
-  <si>
-    <t>logfile_folder</t>
-  </si>
-  <si>
-    <t>summaries_folder</t>
-  </si>
-  <si>
-    <t>simap_database_folder</t>
-  </si>
-  <si>
-    <t>uniprot_folder</t>
-  </si>
-  <si>
     <t>D:\Databases\main\logfiles</t>
   </si>
   <si>
@@ -420,133 +570,10 @@
     <t>D:\Databases\simap</t>
   </si>
   <si>
+    <t>D:\Databases\homol</t>
+  </si>
+  <si>
     <t>D:\Databases\D_uniprot</t>
-  </si>
-  <si>
-    <t>list_of_uniprot_accessions</t>
-  </si>
-  <si>
-    <t>D:\Databases\main\input_acc_lists\List01_uniprot_accessions.txt</t>
-  </si>
-  <si>
-    <t>aa_sub_matrices</t>
-  </si>
-  <si>
-    <t>mp_xlim_min01</t>
-  </si>
-  <si>
-    <t>mp_xlim_max01</t>
-  </si>
-  <si>
-    <t>fa_words_not_allowed_in_description</t>
-  </si>
-  <si>
-    <t>fa_database</t>
-  </si>
-  <si>
-    <t>fa_min_identity_of_TMD_initial_filter</t>
-  </si>
-  <si>
-    <t>fa_min_identity_of_TMD_final_filter</t>
-  </si>
-  <si>
-    <t>fa_identity_method</t>
-  </si>
-  <si>
-    <t>fa_randomised_tmd</t>
-  </si>
-  <si>
-    <t>fa_aa_before_tmd</t>
-  </si>
-  <si>
-    <t>fa_aa_after_tmd</t>
-  </si>
-  <si>
-    <t>fa_X_allowed_in_sel_seq</t>
-  </si>
-  <si>
-    <t>cr_words_not_allowed_in_description</t>
-  </si>
-  <si>
-    <t>cr_database</t>
-  </si>
-  <si>
-    <t>cr_minimum_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>cr_min_identity_of_TMD_initial_filter</t>
-  </si>
-  <si>
-    <t>cr_min_identity_of_TMD_final_filter</t>
-  </si>
-  <si>
-    <t>cr_X_allowed_in_full_seq</t>
-  </si>
-  <si>
-    <t>cr_min_len_query_aln_seq_excl_TMD</t>
-  </si>
-  <si>
-    <t>cr_identity_method</t>
-  </si>
-  <si>
-    <t>cr_maximum_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>cr_mimimum_length_match_sequence</t>
-  </si>
-  <si>
-    <t>cr_mimimum_length_non_TMD_sequence</t>
-  </si>
-  <si>
-    <t>cr_randomised_tmd</t>
-  </si>
-  <si>
-    <t>fa_X_allowed_in_full_seq</t>
-  </si>
-  <si>
-    <t>fa_max_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>fa_min_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>cr_max_n_gaps_in_match_TMD</t>
-  </si>
-  <si>
-    <t>cr_max_n_gaps_in_query_TMD</t>
-  </si>
-  <si>
-    <t>fa_max_n_gaps_in_match_TMD</t>
-  </si>
-  <si>
-    <t>fa_max_n_gaps_in_query_TMD</t>
-  </si>
-  <si>
-    <t>remove_redundant_seqs</t>
-  </si>
-  <si>
-    <t>add_query_seq</t>
-  </si>
-  <si>
-    <t>save_fasta_plus_surr</t>
-  </si>
-  <si>
-    <t>save a second fasta output with the TMD or selected sequence plus the surrounding sequence</t>
-  </si>
-  <si>
-    <t>SIMAP homologue filtering for conservation ratio (cr) output</t>
-  </si>
-  <si>
-    <t>SIMAP homologue filtering for fasta (fa) output</t>
-  </si>
-  <si>
-    <t>filter_selected_seq_based_on_hydrophobicity</t>
-  </si>
-  <si>
-    <t>max_hydrophilicity_Hessa</t>
-  </si>
-  <si>
-    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment.</t>
   </si>
 </sst>
 </file>
@@ -900,7 +927,21 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -996,6 +1037,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1290,32 +1334,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -1325,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="37">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>9</v>
@@ -1358,14 +1402,14 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>8</v>
@@ -1376,7 +1420,7 @@
     </row>
     <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B9" s="70" t="s">
         <v>8</v>
@@ -1387,7 +1431,7 @@
     </row>
     <row r="10" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>8</v>
@@ -1398,7 +1442,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" s="70" t="s">
         <v>8</v>
@@ -1408,91 +1452,91 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>105</v>
+      <c r="A12" s="31" t="s">
+        <v>175</v>
       </c>
       <c r="B12" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="70" t="s">
+      <c r="A13" s="62"/>
+      <c r="C13" s="62"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="57"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C15" s="65" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="C14" s="62"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="57"/>
-    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
-        <v>107</v>
+      <c r="A16" s="66" t="s">
+        <v>103</v>
       </c>
       <c r="B16" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="66" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="66" t="s">
-        <v>19</v>
-      </c>
+      <c r="A17" s="62"/>
+      <c r="C17" s="62"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="C18" s="62"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="59"/>
+      <c r="A18" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="59"/>
+    </row>
+    <row r="19" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>7</v>
+        <v>104</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>8</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B21" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1502,42 +1546,42 @@
     </row>
     <row r="23" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="60"/>
     </row>
     <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B24" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B25" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B26" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,126 +1590,136 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B30" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B31" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B32" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B33" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B34" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B6 B35:B1048576">
-    <cfRule type="containsText" dxfId="11" priority="37" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="90" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="10" priority="35" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="containsText" dxfId="12" priority="88" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="9" priority="34" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B18)))</formula>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="11" priority="87" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="containsText" dxfId="7" priority="32" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="85" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B34 B24 B26 B8:B10 B16">
-    <cfRule type="containsText" dxfId="6" priority="31" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B29:B34 B24 B26 B8:B9">
+    <cfRule type="containsText" dxfId="8" priority="84" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="5" priority="23" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="containsText" dxfId="7" priority="74" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="4" priority="22" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
+  <conditionalFormatting sqref="B15 B10:B12">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17 B11:B13">
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1675,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,56 +1744,56 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -1747,42 +1801,67 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>184</v>
+      </c>
+      <c r="C11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1798,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,25 +1892,25 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>8</v>
@@ -1840,7 +1919,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="37">
         <v>50</v>
@@ -1849,24 +1928,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>27</v>
-      </c>
       <c r="C6" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1875,14 +1954,14 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>7</v>
@@ -1891,16 +1970,16 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="B10" s="40" t="b">
+        <v>0</v>
       </c>
       <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>8</v>
@@ -1909,7 +1988,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>7</v>
@@ -1918,18 +1997,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="40">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="40">
         <v>1.0000000000000001E-5</v>
@@ -1938,7 +2017,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="40">
         <v>5000</v>
@@ -1947,7 +2026,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="40">
         <v>3000</v>
@@ -1956,7 +2035,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>8</v>
@@ -1965,10 +2044,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="56"/>
     </row>
@@ -1978,43 +2057,47 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="57"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="58" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="58" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B23" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>7</v>
@@ -2023,619 +2106,609 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B25" s="42">
         <v>-1</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B26" s="42">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C26" s="58"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B27" s="42">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C27" s="58"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="58"/>
+        <v>34</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B29" s="42">
         <v>0.4</v>
       </c>
-      <c r="C29" s="58"/>
+      <c r="C29" s="58" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B30" s="42">
         <v>1</v>
       </c>
-      <c r="C30" s="58"/>
+      <c r="C30" s="58" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B31" s="42">
-        <v>0.3</v>
+        <v>145</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>7</v>
       </c>
       <c r="C31" s="58"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B32" s="42">
-        <v>0.3</v>
+        <v>132</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="B33" s="42" t="s">
-        <v>8</v>
+        <v>130</v>
+      </c>
+      <c r="B33" s="42">
+        <v>10</v>
       </c>
       <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" s="42" t="s">
-        <v>8</v>
+        <v>131</v>
+      </c>
+      <c r="B34" s="42">
+        <v>10</v>
       </c>
       <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C35" s="58"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="42">
-        <v>10</v>
-      </c>
-      <c r="C36" s="58"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B37" s="42">
-        <v>10</v>
-      </c>
-      <c r="C37" s="58"/>
+        <v>128</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="38"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="42" t="s">
+      <c r="A38" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" s="72"/>
+      <c r="C38" s="73"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="75" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="76"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="76"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="58"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="58"/>
-    </row>
-    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="38"/>
-      <c r="C40" s="8"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="73"/>
+      <c r="C41" s="76"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="B42" s="75" t="s">
-        <v>33</v>
+        <v>148</v>
+      </c>
+      <c r="B42" s="75">
+        <v>2</v>
       </c>
       <c r="C42" s="76"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" s="75" t="s">
-        <v>34</v>
+        <v>149</v>
+      </c>
+      <c r="B43" s="75">
+        <v>2</v>
       </c>
       <c r="C43" s="76"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="B44" s="75">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C44" s="76"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B45" s="75">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="C45" s="76"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B46" s="75">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C46" s="76"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" s="75">
-        <v>0.3</v>
+        <v>138</v>
+      </c>
+      <c r="B47" s="75" t="s">
+        <v>8</v>
       </c>
       <c r="C47" s="76"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B48" s="75">
-        <v>0.3</v>
+        <v>20</v>
       </c>
       <c r="C48" s="76"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B49" s="75" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C49" s="76"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B50" s="75">
-        <v>20</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C50" s="76"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>156</v>
-      </c>
-      <c r="B51" s="75" t="s">
-        <v>35</v>
+        <v>142</v>
+      </c>
+      <c r="B51" s="75">
+        <v>0</v>
       </c>
       <c r="C51" s="76"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B52" s="75">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C52" s="76"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="B53" s="75">
-        <v>0</v>
+        <v>144</v>
+      </c>
+      <c r="B53" s="75" t="s">
+        <v>8</v>
       </c>
       <c r="C53" s="76"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="74" t="s">
-        <v>159</v>
-      </c>
-      <c r="B54" s="75">
-        <v>0</v>
-      </c>
-      <c r="C54" s="76"/>
+    <row r="54" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="38"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="B55" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="76"/>
-    </row>
-    <row r="56" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="38"/>
-      <c r="C56" s="8"/>
+      <c r="A55" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="43"/>
+      <c r="C55" s="59"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="25"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="59"/>
+      <c r="A57" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="44">
+        <v>2</v>
+      </c>
+      <c r="C57" s="25"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="44" t="s">
-        <v>7</v>
+        <v>57</v>
+      </c>
+      <c r="B58" s="44">
+        <v>24</v>
       </c>
       <c r="C58" s="25"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="44">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C59" s="25"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="44">
-        <v>24</v>
-      </c>
-      <c r="C60" s="25"/>
+    <row r="60" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="38"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" s="44">
-        <v>20</v>
-      </c>
-      <c r="C61" s="25"/>
+      <c r="A61" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="45"/>
+      <c r="C61" s="60"/>
     </row>
     <row r="62" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="38"/>
-      <c r="C62" s="8"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+      <c r="A62" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="45"/>
-      <c r="C63" s="60"/>
+      <c r="B62" s="46">
+        <v>30</v>
+      </c>
+      <c r="C62" s="61"/>
+    </row>
+    <row r="63" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="61"/>
     </row>
     <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B64" s="46">
-        <v>30</v>
+        <v>3.05</v>
       </c>
       <c r="C64" s="61"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="46" t="s">
-        <v>7</v>
+        <v>115</v>
+      </c>
+      <c r="B65" s="46">
+        <v>20</v>
       </c>
       <c r="C65" s="61"/>
     </row>
     <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B66" s="46">
-        <v>3.05</v>
+        <v>31</v>
       </c>
       <c r="C66" s="61"/>
     </row>
     <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="46">
-        <v>20</v>
+        <v>84</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C67" s="61"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="46">
-        <v>31</v>
+        <v>85</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>8</v>
       </c>
       <c r="C68" s="61"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="46" t="s">
-        <v>7</v>
+        <v>86</v>
+      </c>
+      <c r="B69" s="46">
+        <v>0.05</v>
       </c>
       <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" s="46" t="s">
-        <v>8</v>
+        <v>87</v>
+      </c>
+      <c r="B70" s="46">
+        <v>3</v>
       </c>
       <c r="C70" s="61"/>
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B71" s="46">
-        <v>0.05</v>
+        <v>88</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C71" s="61"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72" s="46">
-        <v>3</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="C72" s="61"/>
     </row>
     <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" s="46">
+        <v>31</v>
+      </c>
+      <c r="C73" s="61"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B73" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="61"/>
-    </row>
-    <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
+      <c r="B74" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="61"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="46">
-        <v>1.4550000000000001</v>
-      </c>
-      <c r="C74" s="61"/>
-    </row>
-    <row r="75" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="s">
-        <v>93</v>
-      </c>
       <c r="B75" s="46">
-        <v>31</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C75" s="61"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B76" s="46" t="s">
-        <v>8</v>
+        <v>125</v>
+      </c>
+      <c r="B76" s="46">
+        <v>0.5</v>
       </c>
       <c r="C76" s="61"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B77" s="46">
-        <v>0.55500000000000005</v>
+        <v>1.75</v>
       </c>
       <c r="C77" s="61"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B78" s="46">
-        <v>0.5</v>
+        <v>31</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C78" s="61"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B79" s="46">
-        <v>1.75</v>
-      </c>
-      <c r="C79" s="61"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B80" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C80" s="61"/>
-    </row>
-    <row r="82" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B82" s="48"/>
-      <c r="C82" s="27"/>
+    <row r="80" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="48"/>
+      <c r="C80" s="27"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" s="49">
+        <v>0</v>
+      </c>
+      <c r="C81" s="29"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B82" s="49">
+        <v>-12</v>
+      </c>
+      <c r="C82" s="29"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B83" s="49">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C83" s="29"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B84" s="49">
-        <v>-12</v>
+        <v>42</v>
+      </c>
+      <c r="B84" s="49" t="s">
+        <v>47</v>
       </c>
       <c r="C84" s="29"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B85" s="49">
-        <v>-2</v>
+        <v>-0.2</v>
       </c>
       <c r="C85" s="29"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B86" s="49" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B86" s="49">
+        <v>-1</v>
       </c>
       <c r="C86" s="29"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B87" s="49">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="C87" s="29"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B88" s="49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="29"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B89" s="49">
-        <v>-1</v>
+        <v>124</v>
+      </c>
+      <c r="B89" s="49" t="s">
+        <v>48</v>
       </c>
       <c r="C89" s="29"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B90" s="49">
-        <v>0</v>
-      </c>
-      <c r="C90" s="29"/>
-    </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C91" s="29"/>
+      <c r="A91" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B91" s="50"/>
+      <c r="C91" s="30"/>
+    </row>
+    <row r="92" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="33"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="B93" s="50"/>
-      <c r="C93" s="30"/>
-    </row>
-    <row r="94" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93" s="51">
+        <v>5</v>
+      </c>
+      <c r="C93" s="33"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B94" s="51" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C94" s="33"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B95" s="51">
-        <v>5</v>
-      </c>
-      <c r="C95" s="33"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B96" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="C96" s="33"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B97" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C97" s="51"/>
+        <v>117</v>
+      </c>
+      <c r="B95" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">

</xml_diff>